<commit_message>
Chiller sheet updated with results
</commit_message>
<xml_diff>
--- a/MasterData/8. AmortTemplateChiller.xlsx
+++ b/MasterData/8. AmortTemplateChiller.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="59">
   <si>
     <t>AmortTemplateNo</t>
   </si>
@@ -5090,12 +5090,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:L110"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5160,7 +5157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>102</v>
       </c>
@@ -5205,7 +5202,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -5250,7 +5247,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
@@ -5295,7 +5292,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>102</v>
       </c>
@@ -5340,7 +5337,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>102</v>
       </c>
@@ -5385,7 +5382,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>102</v>
       </c>
@@ -5430,7 +5427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>103</v>
       </c>
@@ -5520,7 +5517,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>103</v>
       </c>
@@ -5565,7 +5562,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>103</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>103</v>
       </c>
@@ -5655,7 +5652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>103</v>
       </c>
@@ -5703,7 +5700,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>103</v>
       </c>
@@ -5748,7 +5745,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>103</v>
       </c>
@@ -5793,7 +5790,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>103</v>
       </c>
@@ -5838,7 +5835,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>103</v>
       </c>
@@ -5883,7 +5880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>103</v>
       </c>
@@ -5928,7 +5925,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>103</v>
       </c>
@@ -5973,7 +5970,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>104</v>
       </c>
@@ -6018,7 +6015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>104</v>
       </c>
@@ -6063,7 +6060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>104</v>
       </c>
@@ -6108,7 +6105,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -6153,7 +6150,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>105</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>105</v>
       </c>
@@ -6243,7 +6240,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>105</v>
       </c>
@@ -6288,7 +6285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>107</v>
       </c>
@@ -6336,7 +6333,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>107</v>
       </c>
@@ -6381,7 +6378,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>107</v>
       </c>
@@ -6426,7 +6423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>107</v>
       </c>
@@ -6471,7 +6468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>107</v>
       </c>
@@ -6516,7 +6513,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>108</v>
       </c>
@@ -6561,7 +6558,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>108</v>
       </c>
@@ -6606,7 +6603,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>108</v>
       </c>
@@ -6651,7 +6648,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>108</v>
       </c>
@@ -6696,7 +6693,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>108</v>
       </c>
@@ -6741,7 +6738,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>108</v>
       </c>
@@ -6786,7 +6783,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>108</v>
       </c>
@@ -6831,7 +6828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>109</v>
       </c>
@@ -6876,7 +6873,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>110</v>
       </c>
@@ -6917,12 +6914,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesBio/Clip (E)Original Series</v>
       </c>
-      <c r="N40" t="e">
-        <f>VLOOKUP(M40,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>110</v>
       </c>
@@ -6963,12 +6959,14 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesConcertOriginal Series</v>
       </c>
-      <c r="N41" t="e">
-        <f>VLOOKUP(M41,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>22</v>
+      </c>
+      <c r="O41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>110</v>
       </c>
@@ -7009,12 +7007,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesDocumentaryOriginal Series</v>
       </c>
-      <c r="N42" t="e">
-        <f>VLOOKUP(M42,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>110</v>
       </c>
@@ -7062,7 +7059,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>110</v>
       </c>
@@ -7103,12 +7100,14 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesEventsOriginal Series</v>
       </c>
-      <c r="N44" t="e">
-        <f>VLOOKUP(M44,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>22</v>
+      </c>
+      <c r="O44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>110</v>
       </c>
@@ -7156,7 +7155,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>110</v>
       </c>
@@ -7204,7 +7203,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>110</v>
       </c>
@@ -7245,12 +7244,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesOriginal SeriesOriginal Series</v>
       </c>
-      <c r="N47" t="e">
-        <f>VLOOKUP(M47,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>110</v>
       </c>
@@ -7291,12 +7289,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesPilotOriginal Series</v>
       </c>
-      <c r="N48" t="e">
-        <f>VLOOKUP(M48,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>110</v>
       </c>
@@ -7337,12 +7334,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesSeriesOriginal Series</v>
       </c>
-      <c r="N49" t="e">
-        <f>VLOOKUP(M49,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>110</v>
       </c>
@@ -7383,12 +7379,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesSpecialOriginal Series</v>
       </c>
-      <c r="N50" t="e">
-        <f>VLOOKUP(M50,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>110</v>
       </c>
@@ -7429,12 +7424,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesSportsOriginal Series</v>
       </c>
-      <c r="N51" t="e">
-        <f>VLOOKUP(M51,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>110</v>
       </c>
@@ -7475,12 +7469,11 @@
         <f t="shared" si="0"/>
         <v>110Original SeriesTopicalsOriginal Series</v>
       </c>
-      <c r="N52" t="e">
-        <f>VLOOKUP(M52,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>111</v>
       </c>
@@ -7525,7 +7518,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>111</v>
       </c>
@@ -7570,7 +7563,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>111</v>
       </c>
@@ -7615,7 +7608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>111</v>
       </c>
@@ -7663,7 +7656,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>111</v>
       </c>
@@ -7708,7 +7701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>111</v>
       </c>
@@ -7753,7 +7746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>111</v>
       </c>
@@ -7798,7 +7791,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>111</v>
       </c>
@@ -7843,7 +7836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>111</v>
       </c>
@@ -7888,7 +7881,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>111</v>
       </c>
@@ -7933,7 +7926,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>111</v>
       </c>
@@ -7978,7 +7971,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>111</v>
       </c>
@@ -8023,7 +8016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>111</v>
       </c>
@@ -8068,7 +8061,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>112</v>
       </c>
@@ -8113,7 +8106,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>112</v>
       </c>
@@ -8158,7 +8151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>112</v>
       </c>
@@ -8203,7 +8196,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>112</v>
       </c>
@@ -8251,7 +8244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>112</v>
       </c>
@@ -8296,7 +8289,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>112</v>
       </c>
@@ -8341,7 +8334,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>112</v>
       </c>
@@ -8386,7 +8379,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>112</v>
       </c>
@@ -8431,7 +8424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>112</v>
       </c>
@@ -8476,7 +8469,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>112</v>
       </c>
@@ -8521,7 +8514,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>112</v>
       </c>
@@ -8566,7 +8559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>112</v>
       </c>
@@ -8611,7 +8604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>112</v>
       </c>
@@ -8697,9 +8690,8 @@
         <f t="shared" si="1"/>
         <v>113Original Movies (Anonymous Rex)DocumentaryOriginal Movies</v>
       </c>
-      <c r="N79" t="e">
-        <f>VLOOKUP(M79,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N79" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -8743,9 +8735,8 @@
         <f t="shared" si="1"/>
         <v>113Original Movies (Anonymous Rex)MoviesOriginal Movies</v>
       </c>
-      <c r="N80" t="e">
-        <f>VLOOKUP(M80,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N80" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -8789,12 +8780,14 @@
         <f t="shared" si="1"/>
         <v>113Original Movies (Anonymous Rex)OriginalOriginal Movies</v>
       </c>
-      <c r="N81" t="e">
-        <f>VLOOKUP(M81,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N81" t="s">
+        <v>22</v>
+      </c>
+      <c r="O81" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>113</v>
       </c>
@@ -8839,7 +8832,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>113</v>
       </c>
@@ -8884,7 +8877,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>113</v>
       </c>
@@ -8970,12 +8963,11 @@
         <f t="shared" si="1"/>
         <v>113Original Movies (Anonymous Rex)SeriesOriginal Movies</v>
       </c>
-      <c r="N85" t="e">
-        <f>VLOOKUP(M85,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N85" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>114</v>
       </c>
@@ -9061,9 +9053,8 @@
         <f t="shared" si="1"/>
         <v>115Acquired OriginalsMoviesAcquired Originals</v>
       </c>
-      <c r="N87" t="e">
-        <f>VLOOKUP(M87,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N87" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -9107,9 +9098,8 @@
         <f t="shared" si="1"/>
         <v>115Acquired OriginalsOriginalAcquired Originals</v>
       </c>
-      <c r="N88" t="e">
-        <f>VLOOKUP(M88,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N88" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -9153,9 +9143,8 @@
         <f t="shared" si="1"/>
         <v>115Acquired OriginalsOriginal MiniSeriesAcquired Originals</v>
       </c>
-      <c r="N89" t="e">
-        <f>VLOOKUP(M89,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N89" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -9199,9 +9188,8 @@
         <f t="shared" si="1"/>
         <v>115Acquired OriginalsSeriesAcquired Originals</v>
       </c>
-      <c r="N90" t="e">
-        <f>VLOOKUP(M90,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N90" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -9245,9 +9233,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)Bio/Clip (E)Original Series</v>
       </c>
-      <c r="N91" t="e">
-        <f>VLOOKUP(M91,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N91" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -9291,9 +9278,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)ConcertOriginal Series</v>
       </c>
-      <c r="N92" t="e">
-        <f>VLOOKUP(M92,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N92" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -9337,12 +9323,11 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)DocumentaryOriginal Series</v>
       </c>
-      <c r="N93" t="e">
-        <f>VLOOKUP(M93,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N93" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>116</v>
       </c>
@@ -9431,9 +9416,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)EventsOriginal Series</v>
       </c>
-      <c r="N95" t="e">
-        <f>VLOOKUP(M95,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N95" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -9477,9 +9461,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)MoviesOriginal Series</v>
       </c>
-      <c r="N96" t="e">
-        <f>VLOOKUP(M96,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N96" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -9523,9 +9506,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)OriginalOriginal Series</v>
       </c>
-      <c r="N97" t="e">
-        <f>VLOOKUP(M97,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N97" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -9569,9 +9551,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)Original SeriesOriginal Series</v>
       </c>
-      <c r="N98" t="e">
-        <f>VLOOKUP(M98,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N98" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -9615,9 +9596,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)PilotOriginal Series</v>
       </c>
-      <c r="N99" t="e">
-        <f>VLOOKUP(M99,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N99" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -9661,9 +9641,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)SeriesOriginal Series</v>
       </c>
-      <c r="N100" t="e">
-        <f>VLOOKUP(M100,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N100" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -9707,9 +9686,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)SpecialOriginal Series</v>
       </c>
-      <c r="N101" t="e">
-        <f>VLOOKUP(M101,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N101" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -9753,9 +9731,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)SportsOriginal Series</v>
       </c>
-      <c r="N102" t="e">
-        <f>VLOOKUP(M102,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N102" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -9799,9 +9776,8 @@
         <f t="shared" si="1"/>
         <v>116Syndicated Series - (SCI FI)TopicalsOriginal Series</v>
       </c>
-      <c r="N103" t="e">
-        <f>VLOOKUP(M103,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N103" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -9845,9 +9821,8 @@
         <f t="shared" si="1"/>
         <v>117PilotDocumentaryOriginal Movies</v>
       </c>
-      <c r="N104" t="e">
-        <f>VLOOKUP(M104,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N104" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -9891,9 +9866,8 @@
         <f t="shared" si="1"/>
         <v>117PilotMoviesOriginal Movies</v>
       </c>
-      <c r="N105" t="e">
-        <f>VLOOKUP(M105,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N105" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -9937,9 +9911,8 @@
         <f t="shared" si="1"/>
         <v>117PilotOriginalOriginal Movies</v>
       </c>
-      <c r="N106" t="e">
-        <f>VLOOKUP(M106,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N106" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -9983,9 +9956,8 @@
         <f t="shared" si="1"/>
         <v>117PilotOriginal MiniSeriesOriginal Movies</v>
       </c>
-      <c r="N107" t="e">
-        <f>VLOOKUP(M107,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N107" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -10029,9 +10001,8 @@
         <f t="shared" si="1"/>
         <v>117PilotOriginal SeriesOriginal Movies</v>
       </c>
-      <c r="N108" t="e">
-        <f>VLOOKUP(M108,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N108" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -10075,9 +10046,8 @@
         <f t="shared" si="1"/>
         <v>117PilotPilotOriginal Movies</v>
       </c>
-      <c r="N109" t="e">
-        <f>VLOOKUP(M109,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N109" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -10121,12 +10091,11 @@
         <f t="shared" si="1"/>
         <v>117PilotSeriesOriginal Movies</v>
       </c>
-      <c r="N110" t="e">
-        <f>VLOOKUP(M110,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N110" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>118</v>
       </c>
@@ -10174,7 +10143,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>118</v>
       </c>
@@ -10222,7 +10191,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>118</v>
       </c>
@@ -10270,7 +10239,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>118</v>
       </c>
@@ -10318,7 +10287,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>118</v>
       </c>
@@ -10366,7 +10335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>118</v>
       </c>
@@ -10414,7 +10383,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>118</v>
       </c>
@@ -10462,7 +10431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>118</v>
       </c>
@@ -10510,7 +10479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -10558,7 +10527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -10606,7 +10575,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -10654,7 +10623,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>181</v>
       </c>
@@ -10702,7 +10671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>181</v>
       </c>
@@ -10750,7 +10719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>181</v>
       </c>
@@ -10798,7 +10767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>181</v>
       </c>
@@ -10847,18 +10816,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O125">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="N"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="13">
-      <filters>
-        <filter val="#N/A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -10869,10 +10826,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E65"/>
+    <sheetView topLeftCell="A75" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11549,7 +11506,7 @@
         <v>55</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" ref="F32:F94" si="1">CONCATENATE(A32,B32,C32,D32)</f>
+        <f t="shared" ref="F32:F96" si="1">CONCATENATE(A32,B32,C32,D32)</f>
         <v>111Original Series (Season 2-3)SportsOriginal Series</v>
       </c>
     </row>
@@ -12247,177 +12204,717 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>116</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" t="s">
+        <v>55</v>
+      </c>
       <c r="F66" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)Original SeriesOriginal Series</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>116</v>
+      </c>
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" t="s">
+        <v>55</v>
+      </c>
       <c r="F67" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)ConcertOriginal Series</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>116</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" t="s">
+        <v>55</v>
+      </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)MoviesOriginal Series</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" t="s">
+        <v>55</v>
+      </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>117PilotOriginal SeriesOriginal Movies</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>115</v>
+      </c>
+      <c r="B70" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
+        <v>39</v>
+      </c>
+      <c r="E70" t="s">
+        <v>55</v>
+      </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>115Acquired OriginalsOriginalAcquired Originals</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>115</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" t="s">
+        <v>55</v>
+      </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>115Acquired OriginalsSeriesAcquired Originals</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" t="s">
+        <v>36</v>
+      </c>
+      <c r="E72" t="s">
+        <v>55</v>
+      </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)Bio/Clip (E)Original Series</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>115</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" t="s">
+        <v>55</v>
+      </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>115Acquired OriginalsMoviesAcquired Originals</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>117</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" t="s">
+        <v>55</v>
+      </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>117PilotDocumentaryOriginal Movies</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>113</v>
+      </c>
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E75" t="s">
+        <v>55</v>
+      </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>113Original Movies (Anonymous Rex)SeriesOriginal Movies</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>116</v>
+      </c>
+      <c r="B76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" t="s">
+        <v>36</v>
+      </c>
+      <c r="E76" t="s">
+        <v>55</v>
+      </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)SeriesOriginal Series</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>116</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" t="s">
+        <v>36</v>
+      </c>
+      <c r="E77" t="s">
+        <v>55</v>
+      </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)SportsOriginal Series</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>115</v>
+      </c>
+      <c r="B78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" t="s">
+        <v>39</v>
+      </c>
+      <c r="E78" t="s">
+        <v>55</v>
+      </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>115Acquired OriginalsOriginal MiniSeriesAcquired Originals</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>116</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" t="s">
+        <v>55</v>
+      </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)DocumentaryOriginal Series</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>116</v>
+      </c>
+      <c r="B80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" t="s">
+        <v>55</v>
+      </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+        <v>116Syndicated Series - (SCI FI)SpecialOriginal Series</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>117</v>
+      </c>
+      <c r="B81" t="s">
+        <v>44</v>
+      </c>
+      <c r="C81" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81" t="s">
+        <v>55</v>
+      </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+        <v>117PilotPilotOriginal Movies</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>117</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" t="s">
+        <v>55</v>
+      </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+        <v>117PilotMoviesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>116</v>
+      </c>
+      <c r="B83" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" t="s">
+        <v>55</v>
+      </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+        <v>116Syndicated Series - (SCI FI)TopicalsOriginal Series</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84" t="s">
+        <v>55</v>
+      </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+        <v>110Original SeriesDocumentaryOriginal Series</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>110</v>
+      </c>
+      <c r="B85" t="s">
+        <v>36</v>
+      </c>
+      <c r="C85" t="s">
+        <v>31</v>
+      </c>
+      <c r="D85" t="s">
+        <v>36</v>
+      </c>
+      <c r="E85" t="s">
+        <v>55</v>
+      </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+        <v>110Original SeriesSpecialOriginal Series</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>116</v>
+      </c>
+      <c r="B86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86" t="s">
+        <v>55</v>
+      </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+        <v>116Syndicated Series - (SCI FI)PilotOriginal Series</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>110</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D87" t="s">
+        <v>36</v>
+      </c>
+      <c r="E87" t="s">
+        <v>55</v>
+      </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+        <v>110Original SeriesPilotOriginal Series</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>117</v>
+      </c>
+      <c r="B88" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" t="s">
+        <v>42</v>
+      </c>
+      <c r="E88" t="s">
+        <v>55</v>
+      </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+        <v>117PilotOriginal MiniSeriesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" t="s">
+        <v>30</v>
+      </c>
+      <c r="D89" t="s">
+        <v>42</v>
+      </c>
+      <c r="E89" t="s">
+        <v>55</v>
+      </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+        <v>117PilotSeriesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>113</v>
+      </c>
+      <c r="B90" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E90" t="s">
+        <v>55</v>
+      </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+        <v>113Original Movies (Anonymous Rex)DocumentaryOriginal Movies</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>113</v>
+      </c>
+      <c r="B91" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E91" t="s">
+        <v>55</v>
+      </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+        <v>113Original Movies (Anonymous Rex)MoviesOriginal Movies</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>117</v>
+      </c>
+      <c r="B92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" t="s">
+        <v>42</v>
+      </c>
+      <c r="E92" t="s">
+        <v>55</v>
+      </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+        <v>117PilotOriginalOriginal Movies</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>110</v>
+      </c>
+      <c r="B93" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" t="s">
+        <v>37</v>
+      </c>
+      <c r="D93" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" t="s">
+        <v>55</v>
+      </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+        <v>110Original SeriesSportsOriginal Series</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>116</v>
+      </c>
+      <c r="B94" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" t="s">
+        <v>55</v>
+      </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>116Syndicated Series - (SCI FI)EventsOriginal Series</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>110</v>
+      </c>
+      <c r="B95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95" t="s">
+        <v>55</v>
+      </c>
+      <c r="F95" t="str">
+        <f t="shared" si="1"/>
+        <v>110Original SeriesSeriesOriginal Series</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>116</v>
+      </c>
+      <c r="B96" t="s">
+        <v>51</v>
+      </c>
+      <c r="C96" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96" t="s">
+        <v>36</v>
+      </c>
+      <c r="E96" t="s">
+        <v>55</v>
+      </c>
+      <c r="F96" t="str">
+        <f t="shared" si="1"/>
+        <v>116Syndicated Series - (SCI FI)OriginalOriginal Series</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>110</v>
+      </c>
+      <c r="B97" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" t="s">
+        <v>36</v>
+      </c>
+      <c r="E97" t="s">
+        <v>55</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" ref="F97:F99" si="2">CONCATENATE(A97,B97,C97,D97)</f>
+        <v>110Original SeriesBio/Clip (E)Original Series</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>110</v>
+      </c>
+      <c r="B98" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" t="s">
+        <v>36</v>
+      </c>
+      <c r="E98" t="s">
+        <v>55</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" si="2"/>
+        <v>110Original SeriesOriginal SeriesOriginal Series</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>110</v>
+      </c>
+      <c r="B99" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" t="s">
+        <v>36</v>
+      </c>
+      <c r="E99" t="s">
+        <v>55</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" si="2"/>
+        <v>110Original SeriesTopicalsOriginal Series</v>
       </c>
     </row>
   </sheetData>

</xml_diff>